<commit_message>
fin: initial backend AI analysis process using yuaiSDK
</commit_message>
<xml_diff>
--- a/src/main/resources/网站数据.xlsx
+++ b/src/main/resources/网站数据.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rocs/Desktop/Study/projects/chatbi/chatbi-backend/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CDCBF5-BE92-FD4A-8DA4-288DC13DF1F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{751AD2A4-D91C-B547-89C3-840580675F19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="740" yWindow="500" windowWidth="28060" windowHeight="16020" xr2:uid="{229EEA6E-F8A7-2545-904A-8F0032855BE1}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>日期</t>
   </si>
@@ -117,6 +117,20 @@
   <si>
     <r>
       <t>6号</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>7号</t>
     </r>
     <r>
       <rPr>
@@ -517,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{260829AF-83D5-9D43-A57C-13A2BDCFFDE0}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="23"/>
@@ -588,6 +602,14 @@
         <v>122</v>
       </c>
     </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="3">
+        <v>156</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>